<commit_message>
FMMM Sector Updates (#228)
</commit_message>
<xml_diff>
--- a/_Shared Resources/TopSky/MSAW/TopSkyMSAW Coding Tool.xlsx
+++ b/_Shared Resources/TopSky/MSAW/TopSkyMSAW Coding Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATC Control\0 GitHub\Sector-Files\_Shared Resources\TopSky\MSAW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42C881C-ECE6-41DA-960F-A150C39B5A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC51CF03-E7D5-4E6D-AB32-0D5CD8C3F880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-1770" windowWidth="29040" windowHeight="16440" xr2:uid="{38210610-A239-4B7F-93EB-C9D3CC6058FF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>South Edge</t>
   </si>
@@ -94,22 +94,19 @@
     <t>S026</t>
   </si>
   <si>
-    <t>S028</t>
-  </si>
-  <si>
-    <t>S029</t>
-  </si>
-  <si>
-    <t>E034</t>
-  </si>
-  <si>
-    <t>E032</t>
-  </si>
-  <si>
-    <t>S010</t>
-  </si>
-  <si>
-    <t>E033</t>
+    <t>E047</t>
+  </si>
+  <si>
+    <t>E043</t>
+  </si>
+  <si>
+    <t>E042</t>
+  </si>
+  <si>
+    <t>E045</t>
+  </si>
+  <si>
+    <t>E040</t>
   </si>
 </sst>
 </file>
@@ -474,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A78920B-173E-4272-A085-64BC10408654}">
-  <dimension ref="A2:I21"/>
+  <dimension ref="A2:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +482,7 @@
     <col min="1" max="1" width="59" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -496,331 +493,780 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A7" si="0">"L:"&amp;D3&amp;".00.00:"&amp;E3&amp;".00.00:1:1:"&amp;C3&amp;":"&amp;F3&amp;"00:"&amp;G3&amp;"00:"&amp;H3&amp;"00:"&amp;I3&amp;"00:"&amp;J3&amp;"00:"&amp;K3&amp;"00:"&amp;L3&amp;"00:"&amp;M3&amp;"00:"&amp;N3&amp;"00:"&amp;O3&amp;"00:"&amp;P3&amp;"00:"&amp;Q3&amp;"00:"&amp;R3&amp;"00:"&amp;S3&amp;"00:"&amp;T3&amp;"00:"&amp;U3&amp;"00:"&amp;V3&amp;"00:"&amp;W3&amp;"00:"&amp;X3&amp;"00:"&amp;Y3&amp;"00"</f>
-        <v>L:S010.00.00:E032.00.00:1:1:3:8500:12000:12100:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S011.00.00:E047.00.00:1:1:9:1400:000:000:000:1400:000:000:000:1300:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C3">
         <f>COUNT(F3:AC3)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="G3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>L:S011.00.00:E033.00.00:1:1:2:10900:10300:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S012.00.00:E043.00.00:1:1:9:10100:000:000:000:1400:000:2100:000:1400:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C19" si="1">COUNT(F4:AC4)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G4">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>21</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>L:S012.00.00:E033.00.00:1:1:3:8800:9100:8600:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S013.00.00:E043.00.00:1:1:7:3900:7600:3500:000:000:3000:7200:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="G5">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="H5">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>L:S013.00.00:E032.00.00:1:1:3:7200:8700:7600:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S014.00.00:E042.00.00:1:1:14:3900:3900:7600:7600:3500:3500:11300:11300:3100:000:000:000:000:1300:00:00:00:00:00:00</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="G6">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="H6">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>76</v>
+      </c>
+      <c r="J6">
+        <v>35</v>
+      </c>
+      <c r="K6">
+        <v>35</v>
+      </c>
+      <c r="L6">
+        <v>113</v>
+      </c>
+      <c r="M6">
+        <v>113</v>
+      </c>
+      <c r="N6">
+        <v>31</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>L:S014.00.00:E032.00.00:1:1:4:8100:7900:7900:8100:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S015.00.00:E047.00.00:1:1:4:2500:11800:11300:3800:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="G7">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="H7">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="I7">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>"L:"&amp;D8&amp;".00.00:"&amp;E8&amp;".00.00:1:1:"&amp;C8&amp;":"&amp;F8&amp;"00:"&amp;G8&amp;"00:"&amp;H8&amp;"00:"&amp;I8&amp;"00:"&amp;J8&amp;"00:"&amp;K8&amp;"00:"&amp;L8&amp;"00:"&amp;M8&amp;"00:"&amp;N8&amp;"00:"&amp;O8&amp;"00:"&amp;P8&amp;"00:"&amp;Q8&amp;"00:"&amp;R8&amp;"00:"&amp;S8&amp;"00:"&amp;T8&amp;"00:"&amp;U8&amp;"00:"&amp;V8&amp;"00:"&amp;W8&amp;"00:"&amp;X8&amp;"00:"&amp;Y8&amp;"00"</f>
-        <v>L:S015.00.00:E032.00.00:1:1:4:7900:8200:9600:8200:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S016.00.00:E045.00.00:1:1:11:1600:2300:2900:11800:11800:5300:000:000:000:1300:2400:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="G8">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="H8">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="I8">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="J8">
+        <v>118</v>
+      </c>
+      <c r="K8">
+        <v>53</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>13</v>
+      </c>
+      <c r="P8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" ref="A9:A19" si="2">"L:"&amp;D9&amp;".00.00:"&amp;E9&amp;".00.00:1:1:"&amp;C9&amp;":"&amp;F9&amp;"00:"&amp;G9&amp;"00:"&amp;H9&amp;"00:"&amp;I9&amp;"00:"&amp;J9&amp;"00:"&amp;K9&amp;"00:"&amp;L9&amp;"00:"&amp;M9&amp;"00:"&amp;N9&amp;"00:"&amp;O9&amp;"00:"&amp;P9&amp;"00:"&amp;Q9&amp;"00:"&amp;R9&amp;"00:"&amp;S9&amp;"00:"&amp;T9&amp;"00:"&amp;U9&amp;"00:"&amp;V9&amp;"00:"&amp;W9&amp;"00:"&amp;X9&amp;"00:"&amp;Y9&amp;"00"</f>
-        <v>L:S016.00.00:E033.00.00:1:1:3:7500:8500:12200:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S017.00.00:E043.00.00:1:1:12:1300:3300:3800:2600:5600:5900:5200:1500:000:000:000:2400:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>26</v>
+      </c>
+      <c r="J9">
+        <v>56</v>
+      </c>
+      <c r="K9">
+        <v>59</v>
+      </c>
+      <c r="L9">
+        <v>52</v>
+      </c>
+      <c r="M9">
+        <v>15</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>24</v>
       </c>
-      <c r="F9">
-        <v>75</v>
-      </c>
-      <c r="G9">
-        <v>85</v>
-      </c>
-      <c r="H9">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S017.00.00:E034.00.00:1:1:2:4600:9100:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S018.00.00:E042.00.00:1:1:14:1300:1400:3800:4800:7100:7400:7400:5300:1500:000:000:000:000:2400:00:00:00:00:00:00</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G10">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>38</v>
+      </c>
+      <c r="I10">
+        <v>48</v>
+      </c>
+      <c r="J10">
+        <v>71</v>
+      </c>
+      <c r="K10">
+        <v>74</v>
+      </c>
+      <c r="L10">
+        <v>74</v>
+      </c>
+      <c r="M10">
+        <v>53</v>
+      </c>
+      <c r="N10">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S018.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S019.00.00:E045.00.00:1:1:13:1300:4400:5800:8400:8200:7500:4300:000:000:000:000:000:2400:00:00:00:00:00:00:00</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>44</v>
+      </c>
+      <c r="H11">
+        <v>58</v>
+      </c>
+      <c r="I11">
+        <v>84</v>
+      </c>
+      <c r="J11">
+        <v>82</v>
+      </c>
+      <c r="K11">
+        <v>75</v>
+      </c>
+      <c r="L11">
+        <v>43</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S019.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S020.00.00:E045.00.00:1:1:13:1300:3300:7300:10000:11000:7500:1400:000:000:000:000:000:2600:00:00:00:00:00:00:00</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>33</v>
+      </c>
+      <c r="H12">
+        <v>73</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>110</v>
+      </c>
+      <c r="K12">
+        <v>75</v>
+      </c>
+      <c r="L12">
+        <v>14</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S020.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S021.00.00:E045.00.00:1:1:14:1500:2800:5500:9800:9700:4700:000:000:000:000:000:000:9800:4000:00:00:00:00:00:00</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>28</v>
+      </c>
+      <c r="H13">
+        <v>55</v>
+      </c>
+      <c r="I13">
+        <v>98</v>
+      </c>
+      <c r="J13">
+        <v>97</v>
+      </c>
+      <c r="K13">
+        <v>47</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>98</v>
+      </c>
+      <c r="S13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S021.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S022.00.00:E045.00.00:1:1:14:2700:3300:5500:9800:8900:4700:000:000:000:000:000:000:12400:4000:00:00:00:00:00:00</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>27</v>
+      </c>
+      <c r="G14">
+        <v>33</v>
+      </c>
+      <c r="H14">
+        <v>55</v>
+      </c>
+      <c r="I14">
+        <v>98</v>
+      </c>
+      <c r="J14">
+        <v>89</v>
+      </c>
+      <c r="K14">
+        <v>47</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>124</v>
+      </c>
+      <c r="S14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S022.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S023.00.00:E040.00.00:1:1:17:1400:000:000:4800:5700:5700:11100:8100:1500:000:000:000:000:000:000:000:4000:00:00:00</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>48</v>
+      </c>
+      <c r="J15">
+        <v>57</v>
+      </c>
+      <c r="K15">
+        <v>57</v>
+      </c>
+      <c r="L15">
+        <v>111</v>
+      </c>
+      <c r="M15">
+        <v>81</v>
+      </c>
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S023.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S024.00.00:E040.00.00:1:1:9:1400:1400:000:4800:4800:7400:11100:11100:1500:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="J16">
+        <v>48</v>
+      </c>
+      <c r="K16">
+        <v>74</v>
+      </c>
+      <c r="L16">
+        <v>111</v>
+      </c>
+      <c r="M16">
+        <v>111</v>
+      </c>
+      <c r="N16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S024.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S025.00.00:E043.00.00:1:1:5:1900:3000:7100:8800:8700:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>71</v>
+      </c>
+      <c r="I17">
+        <v>88</v>
+      </c>
+      <c r="J17">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S025.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:S026.00.00:E043.00.00:1:1:5:1900:7100:7100:8800:8800:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>71</v>
+      </c>
+      <c r="H18">
+        <v>71</v>
+      </c>
+      <c r="I18">
+        <v>88</v>
+      </c>
+      <c r="J18">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>L:S026.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
+        <v>L:.00.00:.00.00:1:1:0:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00:00</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>